<commit_message>
update sleep time of blc notification
</commit_message>
<xml_diff>
--- a/balance_notification/balance_limits.xlsx
+++ b/balance_notification/balance_limits.xlsx
@@ -343,7 +343,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="2">
-        <v>3000000.0</v>
+        <v>-1.0</v>
       </c>
       <c r="D2" s="2">
         <v>-1.0</v>
@@ -441,7 +441,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="5">
-        <v>3000000.0</v>
+        <v>-1.0</v>
       </c>
       <c r="D9" s="5">
         <v>-1.0</v>
@@ -494,7 +494,7 @@
         <v>-1.0</v>
       </c>
       <c r="D11" s="2">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="12">

</xml_diff>